<commit_message>
update to release version
</commit_message>
<xml_diff>
--- a/data/interim/crosswalk.xlsx
+++ b/data/interim/crosswalk.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicholashand/LocalWork/DataVisualizations/asbestos-dashboard/asbestos-dashboard-data/data/interim/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1B4C810-3683-1B4C-BF1F-BFF23D06A3C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BBA506B-FE45-A547-B082-4DCDE0451CC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1510" uniqueCount="925">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1510" uniqueCount="924">
   <si>
     <t>facility_name</t>
   </si>
@@ -2414,9 +2414,6 @@
   </si>
   <si>
     <t>Olney Charter High School</t>
-  </si>
-  <si>
-    <t>Olney West High School</t>
   </si>
   <si>
     <t>Overbrook Educational Ctr</t>
@@ -3168,8 +3165,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B755"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A454" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="A468" sqref="A468"/>
+    <sheetView tabSelected="1" topLeftCell="A634" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="B648" sqref="B648"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -8359,36 +8356,36 @@
         <v>797</v>
       </c>
       <c r="B648" t="s">
-        <v>798</v>
+        <v>703</v>
       </c>
     </row>
     <row r="649" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A649" t="s">
+        <v>798</v>
+      </c>
+      <c r="B649" t="s">
         <v>799</v>
-      </c>
-      <c r="B649" t="s">
-        <v>800</v>
       </c>
     </row>
     <row r="650" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A650" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
       <c r="B650" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
     </row>
     <row r="651" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A651" t="s">
-        <v>802</v>
+        <v>801</v>
       </c>
       <c r="B651" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
     </row>
     <row r="652" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A652" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
       <c r="B652" t="s">
         <v>271</v>
@@ -8396,87 +8393,87 @@
     </row>
     <row r="653" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A653" t="s">
+        <v>803</v>
+      </c>
+      <c r="B653" t="s">
         <v>804</v>
-      </c>
-      <c r="B653" t="s">
-        <v>805</v>
       </c>
     </row>
     <row r="654" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A654" t="s">
+        <v>805</v>
+      </c>
+      <c r="B654" t="s">
         <v>806</v>
-      </c>
-      <c r="B654" t="s">
-        <v>807</v>
       </c>
     </row>
     <row r="655" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A655" t="s">
+        <v>807</v>
+      </c>
+      <c r="B655" t="s">
         <v>808</v>
-      </c>
-      <c r="B655" t="s">
-        <v>809</v>
       </c>
     </row>
     <row r="656" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A656" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
       <c r="B656" t="s">
-        <v>809</v>
+        <v>808</v>
       </c>
     </row>
     <row r="657" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A657" t="s">
+        <v>810</v>
+      </c>
+      <c r="B657" t="s">
         <v>811</v>
-      </c>
-      <c r="B657" t="s">
-        <v>812</v>
       </c>
     </row>
     <row r="658" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A658" t="s">
-        <v>813</v>
+        <v>812</v>
       </c>
       <c r="B658" t="s">
-        <v>812</v>
+        <v>811</v>
       </c>
     </row>
     <row r="659" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A659" t="s">
+        <v>813</v>
+      </c>
+      <c r="B659" t="s">
         <v>814</v>
-      </c>
-      <c r="B659" t="s">
-        <v>815</v>
       </c>
     </row>
     <row r="660" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A660" t="s">
+        <v>815</v>
+      </c>
+      <c r="B660" t="s">
         <v>816</v>
-      </c>
-      <c r="B660" t="s">
-        <v>817</v>
       </c>
     </row>
     <row r="661" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A661" t="s">
+        <v>817</v>
+      </c>
+      <c r="B661" t="s">
         <v>818</v>
-      </c>
-      <c r="B661" t="s">
-        <v>819</v>
       </c>
     </row>
     <row r="662" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A662" t="s">
-        <v>820</v>
+        <v>819</v>
       </c>
       <c r="B662" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
     </row>
     <row r="663" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A663" t="s">
-        <v>821</v>
+        <v>820</v>
       </c>
       <c r="B663" t="s">
         <v>519</v>
@@ -8484,15 +8481,15 @@
     </row>
     <row r="664" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A664" t="s">
+        <v>821</v>
+      </c>
+      <c r="B664" t="s">
         <v>822</v>
-      </c>
-      <c r="B664" t="s">
-        <v>823</v>
       </c>
     </row>
     <row r="665" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A665" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B665" t="s">
         <v>35</v>
@@ -8500,7 +8497,7 @@
     </row>
     <row r="666" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A666" t="s">
-        <v>825</v>
+        <v>824</v>
       </c>
       <c r="B666" t="s">
         <v>37</v>
@@ -8508,7 +8505,7 @@
     </row>
     <row r="667" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A667" t="s">
-        <v>826</v>
+        <v>825</v>
       </c>
       <c r="B667" t="s">
         <v>3</v>
@@ -8516,7 +8513,7 @@
     </row>
     <row r="668" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A668" t="s">
-        <v>827</v>
+        <v>826</v>
       </c>
       <c r="B668" t="s">
         <v>81</v>
@@ -8524,7 +8521,7 @@
     </row>
     <row r="669" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A669" t="s">
-        <v>828</v>
+        <v>827</v>
       </c>
       <c r="B669" t="s">
         <v>708</v>
@@ -8532,7 +8529,7 @@
     </row>
     <row r="670" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A670" t="s">
-        <v>829</v>
+        <v>828</v>
       </c>
       <c r="B670" t="s">
         <v>523</v>
@@ -8540,7 +8537,7 @@
     </row>
     <row r="671" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A671" t="s">
-        <v>830</v>
+        <v>829</v>
       </c>
       <c r="B671" t="s">
         <v>44</v>
@@ -8548,7 +8545,7 @@
     </row>
     <row r="672" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A672" t="s">
-        <v>831</v>
+        <v>830</v>
       </c>
       <c r="B672" t="s">
         <v>5</v>
@@ -8556,7 +8553,7 @@
     </row>
     <row r="673" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A673" t="s">
-        <v>832</v>
+        <v>831</v>
       </c>
       <c r="B673" t="s">
         <v>72</v>
@@ -8564,7 +8561,7 @@
     </row>
     <row r="674" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A674" t="s">
-        <v>833</v>
+        <v>832</v>
       </c>
       <c r="B674" t="s">
         <v>140</v>
@@ -8572,7 +8569,7 @@
     </row>
     <row r="675" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A675" t="s">
-        <v>834</v>
+        <v>833</v>
       </c>
       <c r="B675" t="s">
         <v>179</v>
@@ -8580,7 +8577,7 @@
     </row>
     <row r="676" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A676" t="s">
-        <v>835</v>
+        <v>834</v>
       </c>
       <c r="B676" t="s">
         <v>698</v>
@@ -8588,7 +8585,7 @@
     </row>
     <row r="677" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A677" t="s">
-        <v>836</v>
+        <v>835</v>
       </c>
       <c r="B677" t="s">
         <v>374</v>
@@ -8596,7 +8593,7 @@
     </row>
     <row r="678" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A678" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
       <c r="B678" t="s">
         <v>190</v>
@@ -8604,7 +8601,7 @@
     </row>
     <row r="679" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A679" t="s">
-        <v>838</v>
+        <v>837</v>
       </c>
       <c r="B679" t="s">
         <v>575</v>
@@ -8612,7 +8609,7 @@
     </row>
     <row r="680" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A680" t="s">
-        <v>839</v>
+        <v>838</v>
       </c>
       <c r="B680" t="s">
         <v>543</v>
@@ -8620,7 +8617,7 @@
     </row>
     <row r="681" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A681" t="s">
-        <v>840</v>
+        <v>839</v>
       </c>
       <c r="B681" t="s">
         <v>452</v>
@@ -8628,7 +8625,7 @@
     </row>
     <row r="682" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A682" t="s">
-        <v>841</v>
+        <v>840</v>
       </c>
       <c r="B682" t="s">
         <v>509</v>
@@ -8636,7 +8633,7 @@
     </row>
     <row r="683" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A683" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
       <c r="B683" t="s">
         <v>599</v>
@@ -8644,7 +8641,7 @@
     </row>
     <row r="684" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A684" t="s">
-        <v>843</v>
+        <v>842</v>
       </c>
       <c r="B684" t="s">
         <v>49</v>
@@ -8652,31 +8649,31 @@
     </row>
     <row r="685" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A685" t="s">
+        <v>843</v>
+      </c>
+      <c r="B685" t="s">
         <v>844</v>
-      </c>
-      <c r="B685" t="s">
-        <v>845</v>
       </c>
     </row>
     <row r="686" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A686" t="s">
+        <v>845</v>
+      </c>
+      <c r="B686" t="s">
         <v>846</v>
-      </c>
-      <c r="B686" t="s">
-        <v>847</v>
       </c>
     </row>
     <row r="687" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A687" t="s">
-        <v>848</v>
+        <v>847</v>
       </c>
       <c r="B687" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
     </row>
     <row r="688" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A688" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
       <c r="B688" t="s">
         <v>13</v>
@@ -8684,31 +8681,31 @@
     </row>
     <row r="689" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A689" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
       <c r="B689" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
     </row>
     <row r="690" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A690" t="s">
-        <v>851</v>
+        <v>850</v>
       </c>
       <c r="B690" t="s">
-        <v>847</v>
+        <v>846</v>
       </c>
     </row>
     <row r="691" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A691" t="s">
-        <v>852</v>
+        <v>851</v>
       </c>
       <c r="B691" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
     </row>
     <row r="692" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A692" t="s">
-        <v>853</v>
+        <v>852</v>
       </c>
       <c r="B692" t="s">
         <v>728</v>
@@ -8716,7 +8713,7 @@
     </row>
     <row r="693" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A693" t="s">
-        <v>854</v>
+        <v>853</v>
       </c>
       <c r="B693" t="s">
         <v>691</v>
@@ -8724,7 +8721,7 @@
     </row>
     <row r="694" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A694" t="s">
-        <v>855</v>
+        <v>854</v>
       </c>
       <c r="B694" t="s">
         <v>209</v>
@@ -8732,31 +8729,31 @@
     </row>
     <row r="695" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A695" t="s">
+        <v>855</v>
+      </c>
+      <c r="B695" t="s">
         <v>856</v>
-      </c>
-      <c r="B695" t="s">
-        <v>857</v>
       </c>
     </row>
     <row r="696" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A696" t="s">
+        <v>857</v>
+      </c>
+      <c r="B696" t="s">
         <v>858</v>
-      </c>
-      <c r="B696" t="s">
-        <v>859</v>
       </c>
     </row>
     <row r="697" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A697" t="s">
+        <v>859</v>
+      </c>
+      <c r="B697" t="s">
         <v>860</v>
-      </c>
-      <c r="B697" t="s">
-        <v>861</v>
       </c>
     </row>
     <row r="698" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A698" t="s">
-        <v>862</v>
+        <v>861</v>
       </c>
       <c r="B698" t="s">
         <v>69</v>
@@ -8772,7 +8769,7 @@
     </row>
     <row r="700" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A700" t="s">
-        <v>863</v>
+        <v>862</v>
       </c>
       <c r="B700" t="s">
         <v>45</v>
@@ -8780,15 +8777,15 @@
     </row>
     <row r="701" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A701" t="s">
+        <v>863</v>
+      </c>
+      <c r="B701" t="s">
         <v>864</v>
-      </c>
-      <c r="B701" t="s">
-        <v>865</v>
       </c>
     </row>
     <row r="702" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A702" t="s">
-        <v>866</v>
+        <v>865</v>
       </c>
       <c r="B702" t="s">
         <v>617</v>
@@ -8796,7 +8793,7 @@
     </row>
     <row r="703" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A703" t="s">
-        <v>867</v>
+        <v>866</v>
       </c>
       <c r="B703" t="s">
         <v>51</v>
@@ -8804,7 +8801,7 @@
     </row>
     <row r="704" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A704" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
       <c r="B704" t="s">
         <v>51</v>
@@ -8812,31 +8809,31 @@
     </row>
     <row r="705" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A705" t="s">
+        <v>868</v>
+      </c>
+      <c r="B705" t="s">
         <v>869</v>
-      </c>
-      <c r="B705" t="s">
-        <v>870</v>
       </c>
     </row>
     <row r="706" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A706" t="s">
-        <v>871</v>
+        <v>870</v>
       </c>
       <c r="B706" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
     </row>
     <row r="707" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A707" t="s">
-        <v>872</v>
+        <v>871</v>
       </c>
       <c r="B707" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
     </row>
     <row r="708" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A708" t="s">
-        <v>873</v>
+        <v>872</v>
       </c>
       <c r="B708" t="s">
         <v>732</v>
@@ -8844,7 +8841,7 @@
     </row>
     <row r="709" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A709" t="s">
-        <v>874</v>
+        <v>873</v>
       </c>
       <c r="B709" t="s">
         <v>69</v>
@@ -8852,7 +8849,7 @@
     </row>
     <row r="710" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A710" t="s">
-        <v>875</v>
+        <v>874</v>
       </c>
       <c r="B710" t="s">
         <v>3</v>
@@ -8860,47 +8857,47 @@
     </row>
     <row r="711" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A711" t="s">
+        <v>875</v>
+      </c>
+      <c r="B711" t="s">
         <v>876</v>
-      </c>
-      <c r="B711" t="s">
-        <v>877</v>
       </c>
     </row>
     <row r="712" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A712" t="s">
+        <v>877</v>
+      </c>
+      <c r="B712" t="s">
         <v>878</v>
-      </c>
-      <c r="B712" t="s">
-        <v>879</v>
       </c>
     </row>
     <row r="713" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A713" t="s">
-        <v>880</v>
+        <v>879</v>
       </c>
       <c r="B713" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
     </row>
     <row r="714" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A714" t="s">
+        <v>880</v>
+      </c>
+      <c r="B714" t="s">
         <v>881</v>
-      </c>
-      <c r="B714" t="s">
-        <v>882</v>
       </c>
     </row>
     <row r="715" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A715" t="s">
-        <v>883</v>
+        <v>882</v>
       </c>
       <c r="B715" t="s">
-        <v>882</v>
+        <v>881</v>
       </c>
     </row>
     <row r="716" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A716" t="s">
-        <v>884</v>
+        <v>883</v>
       </c>
       <c r="B716" t="s">
         <v>749</v>
@@ -8908,23 +8905,23 @@
     </row>
     <row r="717" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A717" t="s">
-        <v>885</v>
+        <v>884</v>
       </c>
       <c r="B717" t="s">
-        <v>857</v>
+        <v>856</v>
       </c>
     </row>
     <row r="718" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A718" t="s">
-        <v>886</v>
+        <v>885</v>
       </c>
       <c r="B718" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
     </row>
     <row r="719" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A719" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
       <c r="B719" t="s">
         <v>76</v>
@@ -8932,23 +8929,23 @@
     </row>
     <row r="720" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A720" t="s">
+        <v>887</v>
+      </c>
+      <c r="B720" t="s">
         <v>888</v>
-      </c>
-      <c r="B720" t="s">
-        <v>889</v>
       </c>
     </row>
     <row r="721" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A721" t="s">
-        <v>890</v>
+        <v>889</v>
       </c>
       <c r="B721" t="s">
-        <v>870</v>
+        <v>869</v>
       </c>
     </row>
     <row r="722" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A722" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
       <c r="B722" t="s">
         <v>51</v>
@@ -8956,31 +8953,31 @@
     </row>
     <row r="723" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A723" t="s">
-        <v>892</v>
+        <v>891</v>
       </c>
       <c r="B723" t="s">
-        <v>882</v>
+        <v>881</v>
       </c>
     </row>
     <row r="724" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A724" t="s">
-        <v>893</v>
+        <v>892</v>
       </c>
       <c r="B724" t="s">
-        <v>882</v>
+        <v>881</v>
       </c>
     </row>
     <row r="725" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A725" t="s">
-        <v>894</v>
+        <v>893</v>
       </c>
       <c r="B725" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
     </row>
     <row r="726" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A726" t="s">
-        <v>895</v>
+        <v>894</v>
       </c>
       <c r="B726" t="s">
         <v>69</v>
@@ -8988,15 +8985,15 @@
     </row>
     <row r="727" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A727" t="s">
-        <v>896</v>
+        <v>895</v>
       </c>
       <c r="B727" t="s">
-        <v>882</v>
+        <v>881</v>
       </c>
     </row>
     <row r="728" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A728" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
       <c r="B728" t="s">
         <v>57</v>
@@ -9004,7 +9001,7 @@
     </row>
     <row r="729" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A729" t="s">
-        <v>898</v>
+        <v>897</v>
       </c>
       <c r="B729" t="s">
         <v>7</v>
@@ -9012,7 +9009,7 @@
     </row>
     <row r="730" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A730" t="s">
-        <v>899</v>
+        <v>898</v>
       </c>
       <c r="B730" t="s">
         <v>51</v>
@@ -9020,15 +9017,15 @@
     </row>
     <row r="731" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A731" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
       <c r="B731" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
     </row>
     <row r="732" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A732" t="s">
-        <v>901</v>
+        <v>900</v>
       </c>
       <c r="B732" t="s">
         <v>69</v>
@@ -9036,7 +9033,7 @@
     </row>
     <row r="733" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A733" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
       <c r="B733" t="s">
         <v>479</v>
@@ -9044,23 +9041,23 @@
     </row>
     <row r="734" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A734" t="s">
-        <v>903</v>
+        <v>902</v>
       </c>
       <c r="B734" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
     </row>
     <row r="735" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A735" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
       <c r="B735" t="s">
-        <v>882</v>
+        <v>881</v>
       </c>
     </row>
     <row r="736" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A736" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
       <c r="B736" t="s">
         <v>115</v>
@@ -9068,7 +9065,7 @@
     </row>
     <row r="737" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A737" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
       <c r="B737" t="s">
         <v>728</v>
@@ -9076,7 +9073,7 @@
     </row>
     <row r="738" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A738" t="s">
-        <v>907</v>
+        <v>906</v>
       </c>
       <c r="B738" t="s">
         <v>190</v>
@@ -9084,7 +9081,7 @@
     </row>
     <row r="739" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A739" t="s">
-        <v>908</v>
+        <v>907</v>
       </c>
       <c r="B739" t="s">
         <v>51</v>
@@ -9092,7 +9089,7 @@
     </row>
     <row r="740" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A740" t="s">
-        <v>909</v>
+        <v>908</v>
       </c>
       <c r="B740" t="s">
         <v>7</v>
@@ -9100,7 +9097,7 @@
     </row>
     <row r="741" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A741" t="s">
-        <v>910</v>
+        <v>909</v>
       </c>
       <c r="B741" t="s">
         <v>57</v>
@@ -9108,7 +9105,7 @@
     </row>
     <row r="742" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A742" t="s">
-        <v>911</v>
+        <v>910</v>
       </c>
       <c r="B742" t="s">
         <v>57</v>
@@ -9116,15 +9113,15 @@
     </row>
     <row r="743" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A743" t="s">
-        <v>912</v>
+        <v>911</v>
       </c>
       <c r="B743" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
     </row>
     <row r="744" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A744" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
       <c r="B744" t="s">
         <v>153</v>
@@ -9132,47 +9129,47 @@
     </row>
     <row r="745" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A745" t="s">
+        <v>913</v>
+      </c>
+      <c r="B745" t="s">
         <v>914</v>
-      </c>
-      <c r="B745" t="s">
-        <v>915</v>
       </c>
     </row>
     <row r="746" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A746" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
       <c r="B746" t="s">
-        <v>882</v>
+        <v>881</v>
       </c>
     </row>
     <row r="747" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A747" t="s">
-        <v>917</v>
+        <v>916</v>
       </c>
       <c r="B747" t="s">
-        <v>882</v>
+        <v>881</v>
       </c>
     </row>
     <row r="748" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A748" t="s">
-        <v>918</v>
+        <v>917</v>
       </c>
       <c r="B748" t="s">
-        <v>812</v>
+        <v>811</v>
       </c>
     </row>
     <row r="749" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A749" t="s">
-        <v>919</v>
+        <v>918</v>
       </c>
       <c r="B749" t="s">
-        <v>847</v>
+        <v>846</v>
       </c>
     </row>
     <row r="750" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A750" t="s">
-        <v>920</v>
+        <v>919</v>
       </c>
       <c r="B750" t="s">
         <v>64</v>
@@ -9180,7 +9177,7 @@
     </row>
     <row r="751" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A751" t="s">
-        <v>921</v>
+        <v>920</v>
       </c>
       <c r="B751" t="s">
         <v>728</v>
@@ -9188,7 +9185,7 @@
     </row>
     <row r="752" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A752" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="B752" t="s">
         <v>34</v>
@@ -9196,7 +9193,7 @@
     </row>
     <row r="753" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A753" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="B753" t="s">
         <v>71</v>
@@ -9212,7 +9209,7 @@
     </row>
     <row r="755" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A755" t="s">
-        <v>924</v>
+        <v>923</v>
       </c>
       <c r="B755" t="s">
         <v>587</v>

</xml_diff>

<commit_message>
update cross walk after fuzzy match
</commit_message>
<xml_diff>
--- a/data/interim/crosswalk.xlsx
+++ b/data/interim/crosswalk.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicholashand/LocalWork/DataVisualizations/asbestos-dashboard/asbestos-dashboard-data/data/interim/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A2AA1B6-FD48-5E4E-B313-D93D1E92C924}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14FEC6C9-1B7B-F741-9600-00CC44EA710B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1522" uniqueCount="931">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1524" uniqueCount="932">
   <si>
     <t>facility_name</t>
   </si>
@@ -2813,6 +2813,9 @@
   </si>
   <si>
     <t>MAYFAIR ELEMENTARY SCHOOL</t>
+  </si>
+  <si>
+    <t>Mary McLeod Bethune School</t>
   </si>
 </sst>
 </file>
@@ -3184,10 +3187,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B761"/>
+  <dimension ref="A1:B762"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A157" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="A170" sqref="A170"/>
+    <sheetView tabSelected="1" topLeftCell="A348" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="B363" sqref="B362:B363"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -6086,7 +6089,7 @@
     </row>
     <row r="362" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A362" t="s">
-        <v>424</v>
+        <v>931</v>
       </c>
       <c r="B362" t="s">
         <v>425</v>
@@ -6094,7 +6097,7 @@
     </row>
     <row r="363" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A363" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="B363" t="s">
         <v>425</v>
@@ -6102,7 +6105,7 @@
     </row>
     <row r="364" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A364" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="B364" t="s">
         <v>425</v>
@@ -6110,15 +6113,15 @@
     </row>
     <row r="365" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A365" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="B365" t="s">
-        <v>429</v>
+        <v>425</v>
       </c>
     </row>
     <row r="366" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A366" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="B366" t="s">
         <v>429</v>
@@ -6126,7 +6129,7 @@
     </row>
     <row r="367" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A367" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="B367" t="s">
         <v>429</v>
@@ -6134,15 +6137,15 @@
     </row>
     <row r="368" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A368" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="B368" t="s">
-        <v>433</v>
+        <v>429</v>
       </c>
     </row>
     <row r="369" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A369" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="B369" t="s">
         <v>433</v>
@@ -6150,7 +6153,7 @@
     </row>
     <row r="370" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A370" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B370" t="s">
         <v>433</v>
@@ -6158,7 +6161,7 @@
     </row>
     <row r="371" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A371" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B371" t="s">
         <v>433</v>
@@ -6166,15 +6169,15 @@
     </row>
     <row r="372" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A372" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="B372" t="s">
-        <v>438</v>
+        <v>433</v>
       </c>
     </row>
     <row r="373" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A373" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="B373" t="s">
         <v>438</v>
@@ -6182,7 +6185,7 @@
     </row>
     <row r="374" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A374" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="B374" t="s">
         <v>438</v>
@@ -6190,7 +6193,7 @@
     </row>
     <row r="375" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A375" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="B375" t="s">
         <v>438</v>
@@ -6198,15 +6201,15 @@
     </row>
     <row r="376" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A376" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B376" t="s">
-        <v>443</v>
+        <v>438</v>
       </c>
     </row>
     <row r="377" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A377" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="B377" t="s">
         <v>443</v>
@@ -6214,7 +6217,7 @@
     </row>
     <row r="378" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A378" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="B378" t="s">
         <v>443</v>
@@ -6222,7 +6225,7 @@
     </row>
     <row r="379" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A379" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="B379" t="s">
         <v>443</v>
@@ -6230,7 +6233,7 @@
     </row>
     <row r="380" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A380" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="B380" t="s">
         <v>443</v>
@@ -6238,7 +6241,7 @@
     </row>
     <row r="381" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A381" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="B381" t="s">
         <v>443</v>
@@ -6246,7 +6249,7 @@
     </row>
     <row r="382" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A382" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="B382" t="s">
         <v>443</v>
@@ -6254,7 +6257,7 @@
     </row>
     <row r="383" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A383" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="B383" t="s">
         <v>443</v>
@@ -6262,15 +6265,15 @@
     </row>
     <row r="384" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A384" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="B384" t="s">
-        <v>452</v>
+        <v>443</v>
       </c>
     </row>
     <row r="385" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A385" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="B385" t="s">
         <v>452</v>
@@ -6278,7 +6281,7 @@
     </row>
     <row r="386" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A386" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="B386" t="s">
         <v>452</v>
@@ -6286,15 +6289,15 @@
     </row>
     <row r="387" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A387" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="B387" t="s">
-        <v>43</v>
+        <v>452</v>
       </c>
     </row>
     <row r="388" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A388" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="B388" t="s">
         <v>43</v>
@@ -6302,7 +6305,7 @@
     </row>
     <row r="389" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A389" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="B389" t="s">
         <v>43</v>
@@ -6310,7 +6313,7 @@
     </row>
     <row r="390" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A390" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="B390" t="s">
         <v>43</v>
@@ -6318,7 +6321,7 @@
     </row>
     <row r="391" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A391" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="B391" t="s">
         <v>43</v>
@@ -6326,7 +6329,7 @@
     </row>
     <row r="392" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A392" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="B392" t="s">
         <v>43</v>
@@ -6334,7 +6337,7 @@
     </row>
     <row r="393" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A393" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="B393" t="s">
         <v>43</v>
@@ -6342,15 +6345,15 @@
     </row>
     <row r="394" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A394" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="B394" t="s">
-        <v>463</v>
+        <v>43</v>
       </c>
     </row>
     <row r="395" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A395" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="B395" t="s">
         <v>463</v>
@@ -6358,7 +6361,7 @@
     </row>
     <row r="396" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A396" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="B396" t="s">
         <v>463</v>
@@ -6366,7 +6369,7 @@
     </row>
     <row r="397" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A397" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="B397" t="s">
         <v>463</v>
@@ -6374,23 +6377,23 @@
     </row>
     <row r="398" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A398" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="B398" t="s">
-        <v>468</v>
+        <v>463</v>
       </c>
     </row>
     <row r="399" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A399" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="B399" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
     </row>
     <row r="400" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A400" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="B400" t="s">
         <v>470</v>
@@ -6398,7 +6401,7 @@
     </row>
     <row r="401" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A401" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="B401" t="s">
         <v>470</v>
@@ -6406,7 +6409,7 @@
     </row>
     <row r="402" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A402" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="B402" t="s">
         <v>470</v>
@@ -6414,7 +6417,7 @@
     </row>
     <row r="403" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A403" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="B403" t="s">
         <v>470</v>
@@ -6422,7 +6425,7 @@
     </row>
     <row r="404" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A404" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="B404" t="s">
         <v>470</v>
@@ -6430,15 +6433,15 @@
     </row>
     <row r="405" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A405" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="B405" t="s">
-        <v>37</v>
+        <v>470</v>
       </c>
     </row>
     <row r="406" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A406" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="B406" t="s">
         <v>37</v>
@@ -6446,15 +6449,15 @@
     </row>
     <row r="407" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A407" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B407" t="s">
-        <v>479</v>
+        <v>37</v>
       </c>
     </row>
     <row r="408" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A408" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="B408" t="s">
         <v>479</v>
@@ -6462,7 +6465,7 @@
     </row>
     <row r="409" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A409" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="B409" t="s">
         <v>479</v>
@@ -6470,7 +6473,7 @@
     </row>
     <row r="410" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A410" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="B410" t="s">
         <v>479</v>
@@ -6478,7 +6481,7 @@
     </row>
     <row r="411" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A411" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="B411" t="s">
         <v>479</v>
@@ -6486,15 +6489,15 @@
     </row>
     <row r="412" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A412" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="B412" t="s">
-        <v>485</v>
+        <v>479</v>
       </c>
     </row>
     <row r="413" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A413" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="B413" t="s">
         <v>485</v>
@@ -6502,15 +6505,15 @@
     </row>
     <row r="414" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A414" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="B414" t="s">
-        <v>488</v>
+        <v>485</v>
       </c>
     </row>
     <row r="415" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A415" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
       <c r="B415" t="s">
         <v>488</v>
@@ -6518,7 +6521,7 @@
     </row>
     <row r="416" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A416" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="B416" t="s">
         <v>488</v>
@@ -6526,15 +6529,15 @@
     </row>
     <row r="417" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A417" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="B417" t="s">
-        <v>492</v>
+        <v>488</v>
       </c>
     </row>
     <row r="418" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A418" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
       <c r="B418" t="s">
         <v>492</v>
@@ -6542,15 +6545,15 @@
     </row>
     <row r="419" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A419" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="B419" t="s">
-        <v>495</v>
+        <v>492</v>
       </c>
     </row>
     <row r="420" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A420" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="B420" t="s">
         <v>495</v>
@@ -6558,7 +6561,7 @@
     </row>
     <row r="421" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A421" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="B421" t="s">
         <v>495</v>
@@ -6566,15 +6569,15 @@
     </row>
     <row r="422" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A422" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="B422" t="s">
-        <v>499</v>
+        <v>495</v>
       </c>
     </row>
     <row r="423" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A423" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="B423" t="s">
         <v>499</v>
@@ -6582,7 +6585,7 @@
     </row>
     <row r="424" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A424" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="B424" t="s">
         <v>499</v>
@@ -6590,7 +6593,7 @@
     </row>
     <row r="425" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A425" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="B425" t="s">
         <v>499</v>
@@ -6598,15 +6601,15 @@
     </row>
     <row r="426" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A426" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="B426" t="s">
-        <v>504</v>
+        <v>499</v>
       </c>
     </row>
     <row r="427" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A427" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
       <c r="B427" t="s">
         <v>504</v>
@@ -6614,15 +6617,15 @@
     </row>
     <row r="428" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A428" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="B428" t="s">
-        <v>26</v>
+        <v>504</v>
       </c>
     </row>
     <row r="429" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A429" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="B429" t="s">
         <v>26</v>
@@ -6630,15 +6633,15 @@
     </row>
     <row r="430" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A430" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="B430" t="s">
-        <v>509</v>
+        <v>26</v>
       </c>
     </row>
     <row r="431" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A431" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
       <c r="B431" t="s">
         <v>509</v>
@@ -6646,15 +6649,15 @@
     </row>
     <row r="432" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A432" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="B432" t="s">
-        <v>512</v>
+        <v>509</v>
       </c>
     </row>
     <row r="433" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A433" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="B433" t="s">
         <v>512</v>
@@ -6662,7 +6665,7 @@
     </row>
     <row r="434" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A434" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="B434" t="s">
         <v>512</v>
@@ -6670,15 +6673,15 @@
     </row>
     <row r="435" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A435" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="B435" t="s">
-        <v>516</v>
+        <v>512</v>
       </c>
     </row>
     <row r="436" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A436" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
       <c r="B436" t="s">
         <v>516</v>
@@ -6686,15 +6689,15 @@
     </row>
     <row r="437" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A437" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="B437" t="s">
-        <v>519</v>
+        <v>516</v>
       </c>
     </row>
     <row r="438" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A438" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
       <c r="B438" t="s">
         <v>519</v>
@@ -6702,7 +6705,7 @@
     </row>
     <row r="439" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A439" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="B439" t="s">
         <v>519</v>
@@ -6710,15 +6713,15 @@
     </row>
     <row r="440" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A440" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="B440" t="s">
-        <v>523</v>
+        <v>519</v>
       </c>
     </row>
     <row r="441" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A441" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
       <c r="B441" t="s">
         <v>523</v>
@@ -6726,7 +6729,7 @@
     </row>
     <row r="442" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A442" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="B442" t="s">
         <v>523</v>
@@ -6734,7 +6737,7 @@
     </row>
     <row r="443" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A443" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="B443" t="s">
         <v>523</v>
@@ -6742,15 +6745,15 @@
     </row>
     <row r="444" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A444" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="B444" t="s">
-        <v>17</v>
+        <v>523</v>
       </c>
     </row>
     <row r="445" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A445" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="B445" t="s">
         <v>17</v>
@@ -6758,7 +6761,7 @@
     </row>
     <row r="446" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A446" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="B446" t="s">
         <v>17</v>
@@ -6766,7 +6769,7 @@
     </row>
     <row r="447" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A447" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="B447" t="s">
         <v>17</v>
@@ -6774,31 +6777,31 @@
     </row>
     <row r="448" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A448" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="B448" t="s">
-        <v>532</v>
+        <v>17</v>
       </c>
     </row>
     <row r="449" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A449" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="B449" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
     </row>
     <row r="450" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A450" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
       <c r="B450" t="s">
-        <v>495</v>
+        <v>534</v>
       </c>
     </row>
     <row r="451" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A451" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="B451" t="s">
         <v>495</v>
@@ -6806,7 +6809,7 @@
     </row>
     <row r="452" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A452" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="B452" t="s">
         <v>495</v>
@@ -6814,15 +6817,15 @@
     </row>
     <row r="453" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A453" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="B453" t="s">
-        <v>539</v>
+        <v>495</v>
       </c>
     </row>
     <row r="454" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A454" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="B454" t="s">
         <v>539</v>
@@ -6830,7 +6833,7 @@
     </row>
     <row r="455" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A455" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="B455" t="s">
         <v>539</v>
@@ -6838,23 +6841,23 @@
     </row>
     <row r="456" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A456" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="B456" t="s">
-        <v>543</v>
+        <v>539</v>
       </c>
     </row>
     <row r="457" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A457" t="s">
-        <v>544</v>
+        <v>542</v>
       </c>
       <c r="B457" t="s">
-        <v>545</v>
+        <v>543</v>
       </c>
     </row>
     <row r="458" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A458" t="s">
-        <v>546</v>
+        <v>544</v>
       </c>
       <c r="B458" t="s">
         <v>545</v>
@@ -6862,7 +6865,7 @@
     </row>
     <row r="459" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A459" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="B459" t="s">
         <v>545</v>
@@ -6870,7 +6873,7 @@
     </row>
     <row r="460" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A460" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="B460" t="s">
         <v>545</v>
@@ -6878,15 +6881,15 @@
     </row>
     <row r="461" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A461" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="B461" t="s">
-        <v>550</v>
+        <v>545</v>
       </c>
     </row>
     <row r="462" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A462" t="s">
-        <v>551</v>
+        <v>549</v>
       </c>
       <c r="B462" t="s">
         <v>550</v>
@@ -6894,7 +6897,7 @@
     </row>
     <row r="463" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A463" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="B463" t="s">
         <v>550</v>
@@ -6902,7 +6905,7 @@
     </row>
     <row r="464" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A464" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="B464" t="s">
         <v>550</v>
@@ -6910,7 +6913,7 @@
     </row>
     <row r="465" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A465" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="B465" t="s">
         <v>550</v>
@@ -6918,7 +6921,7 @@
     </row>
     <row r="466" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A466" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="B466" t="s">
         <v>550</v>
@@ -6926,7 +6929,7 @@
     </row>
     <row r="467" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A467" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="B467" t="s">
         <v>550</v>
@@ -6934,15 +6937,15 @@
     </row>
     <row r="468" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A468" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="B468" t="s">
-        <v>558</v>
+        <v>550</v>
       </c>
     </row>
     <row r="469" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A469" t="s">
-        <v>559</v>
+        <v>557</v>
       </c>
       <c r="B469" t="s">
         <v>558</v>
@@ -6950,7 +6953,7 @@
     </row>
     <row r="470" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A470" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="B470" t="s">
         <v>558</v>
@@ -6958,7 +6961,7 @@
     </row>
     <row r="471" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A471" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="B471" t="s">
         <v>558</v>
@@ -6966,15 +6969,15 @@
     </row>
     <row r="472" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A472" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="B472" t="s">
-        <v>16</v>
+        <v>558</v>
       </c>
     </row>
     <row r="473" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A473" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="B473" t="s">
         <v>16</v>
@@ -6982,15 +6985,15 @@
     </row>
     <row r="474" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A474" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="B474" t="s">
-        <v>3</v>
+        <v>16</v>
       </c>
     </row>
     <row r="475" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A475" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="B475" t="s">
         <v>3</v>
@@ -6998,15 +7001,15 @@
     </row>
     <row r="476" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A476" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="B476" t="s">
-        <v>64</v>
+        <v>3</v>
       </c>
     </row>
     <row r="477" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A477" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="B477" t="s">
         <v>64</v>
@@ -7014,7 +7017,7 @@
     </row>
     <row r="478" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A478" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="B478" t="s">
         <v>64</v>
@@ -7022,15 +7025,15 @@
     </row>
     <row r="479" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A479" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="B479" t="s">
-        <v>570</v>
+        <v>64</v>
       </c>
     </row>
     <row r="480" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A480" t="s">
-        <v>571</v>
+        <v>569</v>
       </c>
       <c r="B480" t="s">
         <v>570</v>
@@ -7038,23 +7041,23 @@
     </row>
     <row r="481" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A481" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="B481" t="s">
-        <v>573</v>
+        <v>570</v>
       </c>
     </row>
     <row r="482" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A482" t="s">
-        <v>574</v>
+        <v>572</v>
       </c>
       <c r="B482" t="s">
-        <v>575</v>
+        <v>573</v>
       </c>
     </row>
     <row r="483" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A483" t="s">
-        <v>576</v>
+        <v>574</v>
       </c>
       <c r="B483" t="s">
         <v>575</v>
@@ -7062,7 +7065,7 @@
     </row>
     <row r="484" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A484" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="B484" t="s">
         <v>575</v>
@@ -7070,15 +7073,15 @@
     </row>
     <row r="485" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A485" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="B485" t="s">
-        <v>579</v>
+        <v>575</v>
       </c>
     </row>
     <row r="486" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A486" t="s">
-        <v>580</v>
+        <v>578</v>
       </c>
       <c r="B486" t="s">
         <v>579</v>
@@ -7086,7 +7089,7 @@
     </row>
     <row r="487" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A487" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="B487" t="s">
         <v>579</v>
@@ -7094,7 +7097,7 @@
     </row>
     <row r="488" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A488" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="B488" t="s">
         <v>579</v>
@@ -7102,15 +7105,15 @@
     </row>
     <row r="489" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A489" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="B489" t="s">
-        <v>584</v>
+        <v>579</v>
       </c>
     </row>
     <row r="490" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A490" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
       <c r="B490" t="s">
         <v>584</v>
@@ -7118,23 +7121,23 @@
     </row>
     <row r="491" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A491" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="B491" t="s">
-        <v>587</v>
+        <v>584</v>
       </c>
     </row>
     <row r="492" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A492" t="s">
-        <v>588</v>
+        <v>586</v>
       </c>
       <c r="B492" t="s">
-        <v>589</v>
+        <v>587</v>
       </c>
     </row>
     <row r="493" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A493" t="s">
-        <v>590</v>
+        <v>588</v>
       </c>
       <c r="B493" t="s">
         <v>589</v>
@@ -7142,7 +7145,7 @@
     </row>
     <row r="494" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A494" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="B494" t="s">
         <v>589</v>
@@ -7150,7 +7153,7 @@
     </row>
     <row r="495" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A495" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="B495" t="s">
         <v>589</v>
@@ -7158,7 +7161,7 @@
     </row>
     <row r="496" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A496" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="B496" t="s">
         <v>589</v>
@@ -7166,7 +7169,7 @@
     </row>
     <row r="497" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A497" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="B497" t="s">
         <v>589</v>
@@ -7174,15 +7177,15 @@
     </row>
     <row r="498" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A498" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="B498" t="s">
-        <v>45</v>
+        <v>589</v>
       </c>
     </row>
     <row r="499" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A499" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="B499" t="s">
         <v>45</v>
@@ -7190,7 +7193,7 @@
     </row>
     <row r="500" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A500" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="B500" t="s">
         <v>45</v>
@@ -7198,15 +7201,15 @@
     </row>
     <row r="501" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A501" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="B501" t="s">
-        <v>599</v>
+        <v>45</v>
       </c>
     </row>
     <row r="502" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A502" t="s">
-        <v>600</v>
+        <v>598</v>
       </c>
       <c r="B502" t="s">
         <v>599</v>
@@ -7214,15 +7217,15 @@
     </row>
     <row r="503" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A503" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="B503" t="s">
-        <v>602</v>
+        <v>599</v>
       </c>
     </row>
     <row r="504" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A504" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="B504" t="s">
         <v>602</v>
@@ -7230,7 +7233,7 @@
     </row>
     <row r="505" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A505" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="B505" t="s">
         <v>602</v>
@@ -7238,7 +7241,7 @@
     </row>
     <row r="506" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A506" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="B506" t="s">
         <v>602</v>
@@ -7246,7 +7249,7 @@
     </row>
     <row r="507" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A507" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="B507" t="s">
         <v>602</v>
@@ -7254,7 +7257,7 @@
     </row>
     <row r="508" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A508" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="B508" t="s">
         <v>602</v>
@@ -7262,7 +7265,7 @@
     </row>
     <row r="509" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A509" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="B509" t="s">
         <v>602</v>
@@ -7270,15 +7273,15 @@
     </row>
     <row r="510" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A510" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="B510" t="s">
-        <v>13</v>
+        <v>602</v>
       </c>
     </row>
     <row r="511" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A511" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="B511" t="s">
         <v>13</v>
@@ -7286,15 +7289,15 @@
     </row>
     <row r="512" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A512" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="B512" t="s">
-        <v>67</v>
+        <v>13</v>
       </c>
     </row>
     <row r="513" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A513" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="B513" t="s">
         <v>67</v>
@@ -7302,15 +7305,15 @@
     </row>
     <row r="514" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A514" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="B514" t="s">
-        <v>46</v>
+        <v>67</v>
       </c>
     </row>
     <row r="515" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A515" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="B515" t="s">
         <v>46</v>
@@ -7318,7 +7321,7 @@
     </row>
     <row r="516" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A516" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="B516" t="s">
         <v>46</v>
@@ -7326,15 +7329,15 @@
     </row>
     <row r="517" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A517" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="B517" t="s">
-        <v>617</v>
+        <v>46</v>
       </c>
     </row>
     <row r="518" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A518" t="s">
-        <v>618</v>
+        <v>616</v>
       </c>
       <c r="B518" t="s">
         <v>617</v>
@@ -7342,15 +7345,15 @@
     </row>
     <row r="519" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A519" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="B519" t="s">
-        <v>620</v>
+        <v>617</v>
       </c>
     </row>
     <row r="520" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A520" t="s">
-        <v>621</v>
+        <v>619</v>
       </c>
       <c r="B520" t="s">
         <v>620</v>
@@ -7358,15 +7361,15 @@
     </row>
     <row r="521" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A521" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="B521" t="s">
-        <v>623</v>
+        <v>620</v>
       </c>
     </row>
     <row r="522" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A522" t="s">
-        <v>624</v>
+        <v>622</v>
       </c>
       <c r="B522" t="s">
         <v>623</v>
@@ -7374,7 +7377,7 @@
     </row>
     <row r="523" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A523" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="B523" t="s">
         <v>623</v>
@@ -7382,23 +7385,23 @@
     </row>
     <row r="524" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A524" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="B524" t="s">
-        <v>627</v>
+        <v>623</v>
       </c>
     </row>
     <row r="525" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A525" t="s">
-        <v>628</v>
+        <v>626</v>
       </c>
       <c r="B525" t="s">
-        <v>11</v>
+        <v>627</v>
       </c>
     </row>
     <row r="526" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A526" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="B526" t="s">
         <v>11</v>
@@ -7406,15 +7409,15 @@
     </row>
     <row r="527" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A527" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="B527" t="s">
-        <v>631</v>
+        <v>11</v>
       </c>
     </row>
     <row r="528" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A528" t="s">
-        <v>632</v>
+        <v>630</v>
       </c>
       <c r="B528" t="s">
         <v>631</v>
@@ -7422,15 +7425,15 @@
     </row>
     <row r="529" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A529" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="B529" t="s">
-        <v>634</v>
+        <v>631</v>
       </c>
     </row>
     <row r="530" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A530" t="s">
-        <v>635</v>
+        <v>633</v>
       </c>
       <c r="B530" t="s">
         <v>634</v>
@@ -7438,7 +7441,7 @@
     </row>
     <row r="531" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A531" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="B531" t="s">
         <v>634</v>
@@ -7446,15 +7449,15 @@
     </row>
     <row r="532" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A532" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="B532" t="s">
-        <v>638</v>
+        <v>634</v>
       </c>
     </row>
     <row r="533" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A533" t="s">
-        <v>639</v>
+        <v>637</v>
       </c>
       <c r="B533" t="s">
         <v>638</v>
@@ -7462,7 +7465,7 @@
     </row>
     <row r="534" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A534" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="B534" t="s">
         <v>638</v>
@@ -7470,31 +7473,31 @@
     </row>
     <row r="535" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A535" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="B535" t="s">
-        <v>642</v>
+        <v>638</v>
       </c>
     </row>
     <row r="536" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A536" t="s">
-        <v>643</v>
+        <v>641</v>
       </c>
       <c r="B536" t="s">
-        <v>40</v>
+        <v>642</v>
       </c>
     </row>
     <row r="537" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A537" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="B537" t="s">
-        <v>645</v>
+        <v>40</v>
       </c>
     </row>
     <row r="538" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A538" t="s">
-        <v>646</v>
+        <v>644</v>
       </c>
       <c r="B538" t="s">
         <v>645</v>
@@ -7502,7 +7505,7 @@
     </row>
     <row r="539" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A539" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="B539" t="s">
         <v>645</v>
@@ -7510,15 +7513,15 @@
     </row>
     <row r="540" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A540" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="B540" t="s">
-        <v>19</v>
+        <v>645</v>
       </c>
     </row>
     <row r="541" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A541" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="B541" t="s">
         <v>19</v>
@@ -7526,7 +7529,7 @@
     </row>
     <row r="542" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A542" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="B542" t="s">
         <v>19</v>
@@ -7534,7 +7537,7 @@
     </row>
     <row r="543" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A543" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="B543" t="s">
         <v>19</v>
@@ -7542,7 +7545,7 @@
     </row>
     <row r="544" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A544" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="B544" t="s">
         <v>19</v>
@@ -7550,23 +7553,23 @@
     </row>
     <row r="545" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A545" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="B545" t="s">
-        <v>59</v>
+        <v>19</v>
       </c>
     </row>
     <row r="546" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A546" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="B546" t="s">
-        <v>23</v>
+        <v>59</v>
       </c>
     </row>
     <row r="547" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A547" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="B547" t="s">
         <v>23</v>
@@ -7574,7 +7577,7 @@
     </row>
     <row r="548" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A548" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="B548" t="s">
         <v>23</v>
@@ -7582,15 +7585,15 @@
     </row>
     <row r="549" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A549" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="B549" t="s">
-        <v>658</v>
+        <v>23</v>
       </c>
     </row>
     <row r="550" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A550" t="s">
-        <v>659</v>
+        <v>657</v>
       </c>
       <c r="B550" t="s">
         <v>658</v>
@@ -7598,15 +7601,15 @@
     </row>
     <row r="551" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A551" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="B551" t="s">
-        <v>661</v>
+        <v>658</v>
       </c>
     </row>
     <row r="552" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A552" t="s">
-        <v>662</v>
+        <v>660</v>
       </c>
       <c r="B552" t="s">
         <v>661</v>
@@ -7614,7 +7617,7 @@
     </row>
     <row r="553" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A553" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="B553" t="s">
         <v>661</v>
@@ -7622,39 +7625,39 @@
     </row>
     <row r="554" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A554" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="B554" t="s">
-        <v>665</v>
+        <v>661</v>
       </c>
     </row>
     <row r="555" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A555" t="s">
-        <v>666</v>
+        <v>664</v>
       </c>
       <c r="B555" t="s">
-        <v>667</v>
+        <v>665</v>
       </c>
     </row>
     <row r="556" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A556" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="B556" t="s">
-        <v>669</v>
+        <v>667</v>
       </c>
     </row>
     <row r="557" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A557" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="B557" t="s">
-        <v>671</v>
+        <v>669</v>
       </c>
     </row>
     <row r="558" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A558" t="s">
-        <v>672</v>
+        <v>670</v>
       </c>
       <c r="B558" t="s">
         <v>671</v>
@@ -7662,7 +7665,7 @@
     </row>
     <row r="559" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A559" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="B559" t="s">
         <v>671</v>
@@ -7670,15 +7673,15 @@
     </row>
     <row r="560" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A560" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="B560" t="s">
-        <v>39</v>
+        <v>671</v>
       </c>
     </row>
     <row r="561" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A561" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="B561" t="s">
         <v>39</v>
@@ -7686,7 +7689,7 @@
     </row>
     <row r="562" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A562" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="B562" t="s">
         <v>39</v>
@@ -7694,7 +7697,7 @@
     </row>
     <row r="563" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A563" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
       <c r="B563" t="s">
         <v>39</v>
@@ -7702,15 +7705,15 @@
     </row>
     <row r="564" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A564" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="B564" t="s">
-        <v>679</v>
+        <v>39</v>
       </c>
     </row>
     <row r="565" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A565" t="s">
-        <v>680</v>
+        <v>678</v>
       </c>
       <c r="B565" t="s">
         <v>679</v>
@@ -7718,7 +7721,7 @@
     </row>
     <row r="566" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A566" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="B566" t="s">
         <v>679</v>
@@ -7726,7 +7729,7 @@
     </row>
     <row r="567" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A567" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="B567" t="s">
         <v>679</v>
@@ -7734,7 +7737,7 @@
     </row>
     <row r="568" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A568" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="B568" t="s">
         <v>679</v>
@@ -7742,23 +7745,23 @@
     </row>
     <row r="569" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A569" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="B569" t="s">
-        <v>685</v>
+        <v>679</v>
       </c>
     </row>
     <row r="570" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A570" t="s">
-        <v>686</v>
+        <v>684</v>
       </c>
       <c r="B570" t="s">
-        <v>687</v>
+        <v>685</v>
       </c>
     </row>
     <row r="571" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A571" t="s">
-        <v>688</v>
+        <v>686</v>
       </c>
       <c r="B571" t="s">
         <v>687</v>
@@ -7766,7 +7769,7 @@
     </row>
     <row r="572" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A572" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="B572" t="s">
         <v>687</v>
@@ -7774,15 +7777,15 @@
     </row>
     <row r="573" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A573" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="B573" t="s">
-        <v>691</v>
+        <v>687</v>
       </c>
     </row>
     <row r="574" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A574" t="s">
-        <v>692</v>
+        <v>690</v>
       </c>
       <c r="B574" t="s">
         <v>691</v>
@@ -7790,39 +7793,39 @@
     </row>
     <row r="575" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A575" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="B575" t="s">
-        <v>694</v>
+        <v>691</v>
       </c>
     </row>
     <row r="576" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A576" t="s">
-        <v>695</v>
+        <v>693</v>
       </c>
       <c r="B576" t="s">
-        <v>696</v>
+        <v>694</v>
       </c>
     </row>
     <row r="577" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A577" t="s">
-        <v>697</v>
+        <v>695</v>
       </c>
       <c r="B577" t="s">
-        <v>698</v>
+        <v>696</v>
       </c>
     </row>
     <row r="578" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A578" t="s">
-        <v>699</v>
+        <v>697</v>
       </c>
       <c r="B578" t="s">
-        <v>700</v>
+        <v>698</v>
       </c>
     </row>
     <row r="579" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A579" t="s">
-        <v>701</v>
+        <v>699</v>
       </c>
       <c r="B579" t="s">
         <v>700</v>
@@ -7830,23 +7833,23 @@
     </row>
     <row r="580" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A580" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="B580" t="s">
-        <v>703</v>
+        <v>700</v>
       </c>
     </row>
     <row r="581" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A581" t="s">
-        <v>704</v>
+        <v>702</v>
       </c>
       <c r="B581" t="s">
-        <v>705</v>
+        <v>703</v>
       </c>
     </row>
     <row r="582" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A582" t="s">
-        <v>706</v>
+        <v>704</v>
       </c>
       <c r="B582" t="s">
         <v>705</v>
@@ -7854,15 +7857,15 @@
     </row>
     <row r="583" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A583" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="B583" t="s">
-        <v>708</v>
+        <v>705</v>
       </c>
     </row>
     <row r="584" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A584" t="s">
-        <v>709</v>
+        <v>707</v>
       </c>
       <c r="B584" t="s">
         <v>708</v>
@@ -7870,15 +7873,15 @@
     </row>
     <row r="585" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A585" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="B585" t="s">
-        <v>711</v>
+        <v>708</v>
       </c>
     </row>
     <row r="586" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A586" t="s">
-        <v>712</v>
+        <v>710</v>
       </c>
       <c r="B586" t="s">
         <v>711</v>
@@ -7886,15 +7889,15 @@
     </row>
     <row r="587" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A587" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
       <c r="B587" t="s">
-        <v>714</v>
+        <v>711</v>
       </c>
     </row>
     <row r="588" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A588" t="s">
-        <v>715</v>
+        <v>713</v>
       </c>
       <c r="B588" t="s">
         <v>714</v>
@@ -7902,7 +7905,7 @@
     </row>
     <row r="589" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A589" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="B589" t="s">
         <v>714</v>
@@ -7910,7 +7913,7 @@
     </row>
     <row r="590" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A590" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
       <c r="B590" t="s">
         <v>714</v>
@@ -7918,7 +7921,7 @@
     </row>
     <row r="591" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A591" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="B591" t="s">
         <v>714</v>
@@ -7926,15 +7929,15 @@
     </row>
     <row r="592" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A592" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
       <c r="B592" t="s">
-        <v>32</v>
+        <v>714</v>
       </c>
     </row>
     <row r="593" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A593" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B593" t="s">
         <v>32</v>
@@ -7942,23 +7945,23 @@
     </row>
     <row r="594" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A594" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
       <c r="B594" t="s">
-        <v>722</v>
+        <v>32</v>
       </c>
     </row>
     <row r="595" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A595" t="s">
-        <v>723</v>
+        <v>721</v>
       </c>
       <c r="B595" t="s">
-        <v>724</v>
+        <v>722</v>
       </c>
     </row>
     <row r="596" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A596" t="s">
-        <v>725</v>
+        <v>723</v>
       </c>
       <c r="B596" t="s">
         <v>724</v>
@@ -7966,23 +7969,23 @@
     </row>
     <row r="597" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A597" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="B597" t="s">
-        <v>206</v>
+        <v>724</v>
       </c>
     </row>
     <row r="598" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A598" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="B598" t="s">
-        <v>728</v>
+        <v>206</v>
       </c>
     </row>
     <row r="599" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A599" t="s">
-        <v>729</v>
+        <v>727</v>
       </c>
       <c r="B599" t="s">
         <v>728</v>
@@ -7990,7 +7993,7 @@
     </row>
     <row r="600" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A600" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="B600" t="s">
         <v>728</v>
@@ -7998,15 +8001,15 @@
     </row>
     <row r="601" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A601" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
       <c r="B601" t="s">
-        <v>732</v>
+        <v>728</v>
       </c>
     </row>
     <row r="602" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A602" t="s">
-        <v>733</v>
+        <v>731</v>
       </c>
       <c r="B602" t="s">
         <v>732</v>
@@ -8014,15 +8017,15 @@
     </row>
     <row r="603" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A603" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="B603" t="s">
-        <v>735</v>
+        <v>732</v>
       </c>
     </row>
     <row r="604" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A604" t="s">
-        <v>736</v>
+        <v>734</v>
       </c>
       <c r="B604" t="s">
         <v>735</v>
@@ -8030,7 +8033,7 @@
     </row>
     <row r="605" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A605" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="B605" t="s">
         <v>735</v>
@@ -8038,7 +8041,7 @@
     </row>
     <row r="606" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A606" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="B606" t="s">
         <v>735</v>
@@ -8046,7 +8049,7 @@
     </row>
     <row r="607" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A607" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
       <c r="B607" t="s">
         <v>735</v>
@@ -8054,15 +8057,15 @@
     </row>
     <row r="608" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A608" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
       <c r="B608" t="s">
-        <v>741</v>
+        <v>735</v>
       </c>
     </row>
     <row r="609" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A609" t="s">
-        <v>742</v>
+        <v>740</v>
       </c>
       <c r="B609" t="s">
         <v>741</v>
@@ -8070,7 +8073,7 @@
     </row>
     <row r="610" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A610" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
       <c r="B610" t="s">
         <v>741</v>
@@ -8078,7 +8081,7 @@
     </row>
     <row r="611" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A611" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="B611" t="s">
         <v>741</v>
@@ -8086,15 +8089,15 @@
     </row>
     <row r="612" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A612" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
       <c r="B612" t="s">
-        <v>746</v>
+        <v>741</v>
       </c>
     </row>
     <row r="613" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A613" t="s">
-        <v>747</v>
+        <v>745</v>
       </c>
       <c r="B613" t="s">
         <v>746</v>
@@ -8102,15 +8105,15 @@
     </row>
     <row r="614" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A614" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
       <c r="B614" t="s">
-        <v>749</v>
+        <v>746</v>
       </c>
     </row>
     <row r="615" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A615" t="s">
-        <v>750</v>
+        <v>748</v>
       </c>
       <c r="B615" t="s">
         <v>749</v>
@@ -8118,7 +8121,7 @@
     </row>
     <row r="616" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A616" t="s">
-        <v>751</v>
+        <v>750</v>
       </c>
       <c r="B616" t="s">
         <v>749</v>
@@ -8126,7 +8129,7 @@
     </row>
     <row r="617" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A617" t="s">
-        <v>752</v>
+        <v>751</v>
       </c>
       <c r="B617" t="s">
         <v>749</v>
@@ -8134,15 +8137,15 @@
     </row>
     <row r="618" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A618" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
       <c r="B618" t="s">
-        <v>754</v>
+        <v>749</v>
       </c>
     </row>
     <row r="619" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A619" t="s">
-        <v>755</v>
+        <v>753</v>
       </c>
       <c r="B619" t="s">
         <v>754</v>
@@ -8150,7 +8153,7 @@
     </row>
     <row r="620" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A620" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
       <c r="B620" t="s">
         <v>754</v>
@@ -8158,7 +8161,7 @@
     </row>
     <row r="621" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A621" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
       <c r="B621" t="s">
         <v>754</v>
@@ -8166,7 +8169,7 @@
     </row>
     <row r="622" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A622" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
       <c r="B622" t="s">
         <v>754</v>
@@ -8174,7 +8177,7 @@
     </row>
     <row r="623" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A623" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
       <c r="B623" t="s">
         <v>754</v>
@@ -8182,7 +8185,7 @@
     </row>
     <row r="624" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A624" t="s">
-        <v>760</v>
+        <v>759</v>
       </c>
       <c r="B624" t="s">
         <v>754</v>
@@ -8190,15 +8193,15 @@
     </row>
     <row r="625" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A625" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="B625" t="s">
-        <v>762</v>
+        <v>754</v>
       </c>
     </row>
     <row r="626" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A626" t="s">
-        <v>763</v>
+        <v>761</v>
       </c>
       <c r="B626" t="s">
         <v>762</v>
@@ -8206,47 +8209,47 @@
     </row>
     <row r="627" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A627" t="s">
-        <v>764</v>
+        <v>763</v>
       </c>
       <c r="B627" t="s">
-        <v>765</v>
+        <v>762</v>
       </c>
     </row>
     <row r="628" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A628" t="s">
-        <v>766</v>
+        <v>764</v>
       </c>
       <c r="B628" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
     </row>
     <row r="629" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A629" t="s">
-        <v>768</v>
+        <v>766</v>
       </c>
       <c r="B629" t="s">
-        <v>769</v>
+        <v>767</v>
       </c>
     </row>
     <row r="630" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A630" t="s">
-        <v>770</v>
+        <v>768</v>
       </c>
       <c r="B630" t="s">
-        <v>771</v>
+        <v>769</v>
       </c>
     </row>
     <row r="631" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A631" t="s">
-        <v>772</v>
+        <v>770</v>
       </c>
       <c r="B631" t="s">
-        <v>773</v>
+        <v>771</v>
       </c>
     </row>
     <row r="632" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A632" t="s">
-        <v>774</v>
+        <v>772</v>
       </c>
       <c r="B632" t="s">
         <v>773</v>
@@ -8254,23 +8257,23 @@
     </row>
     <row r="633" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A633" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
       <c r="B633" t="s">
-        <v>776</v>
+        <v>773</v>
       </c>
     </row>
     <row r="634" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A634" t="s">
-        <v>777</v>
+        <v>775</v>
       </c>
       <c r="B634" t="s">
-        <v>778</v>
+        <v>776</v>
       </c>
     </row>
     <row r="635" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A635" t="s">
-        <v>779</v>
+        <v>777</v>
       </c>
       <c r="B635" t="s">
         <v>778</v>
@@ -8278,23 +8281,23 @@
     </row>
     <row r="636" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A636" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
       <c r="B636" t="s">
-        <v>781</v>
+        <v>778</v>
       </c>
     </row>
     <row r="637" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A637" t="s">
-        <v>782</v>
+        <v>780</v>
       </c>
       <c r="B637" t="s">
-        <v>783</v>
+        <v>781</v>
       </c>
     </row>
     <row r="638" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A638" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="B638" t="s">
         <v>783</v>
@@ -8302,23 +8305,23 @@
     </row>
     <row r="639" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A639" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="B639" t="s">
-        <v>786</v>
+        <v>783</v>
       </c>
     </row>
     <row r="640" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A640" t="s">
-        <v>787</v>
+        <v>785</v>
       </c>
       <c r="B640" t="s">
-        <v>34</v>
+        <v>786</v>
       </c>
     </row>
     <row r="641" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A641" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
       <c r="B641" t="s">
         <v>34</v>
@@ -8326,7 +8329,7 @@
     </row>
     <row r="642" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A642" t="s">
-        <v>789</v>
+        <v>788</v>
       </c>
       <c r="B642" t="s">
         <v>34</v>
@@ -8334,7 +8337,7 @@
     </row>
     <row r="643" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A643" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
       <c r="B643" t="s">
         <v>34</v>
@@ -8342,7 +8345,7 @@
     </row>
     <row r="644" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A644" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
       <c r="B644" t="s">
         <v>34</v>
@@ -8350,23 +8353,23 @@
     </row>
     <row r="645" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A645" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="B645" t="s">
-        <v>793</v>
+        <v>34</v>
       </c>
     </row>
     <row r="646" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A646" t="s">
-        <v>794</v>
+        <v>792</v>
       </c>
       <c r="B646" t="s">
-        <v>7</v>
+        <v>793</v>
       </c>
     </row>
     <row r="647" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A647" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
       <c r="B647" t="s">
         <v>7</v>
@@ -8374,7 +8377,7 @@
     </row>
     <row r="648" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A648" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
       <c r="B648" t="s">
         <v>7</v>
@@ -8382,31 +8385,31 @@
     </row>
     <row r="649" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A649" t="s">
-        <v>609</v>
+        <v>796</v>
       </c>
       <c r="B649" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
     </row>
     <row r="650" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A650" t="s">
-        <v>797</v>
+        <v>609</v>
       </c>
       <c r="B650" t="s">
-        <v>703</v>
+        <v>13</v>
       </c>
     </row>
     <row r="651" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A651" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
       <c r="B651" t="s">
-        <v>799</v>
+        <v>703</v>
       </c>
     </row>
     <row r="652" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A652" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="B652" t="s">
         <v>799</v>
@@ -8414,7 +8417,7 @@
     </row>
     <row r="653" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A653" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
       <c r="B653" t="s">
         <v>799</v>
@@ -8422,39 +8425,39 @@
     </row>
     <row r="654" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A654" t="s">
-        <v>802</v>
+        <v>801</v>
       </c>
       <c r="B654" t="s">
-        <v>271</v>
+        <v>799</v>
       </c>
     </row>
     <row r="655" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A655" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
       <c r="B655" t="s">
-        <v>804</v>
+        <v>271</v>
       </c>
     </row>
     <row r="656" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A656" t="s">
-        <v>805</v>
+        <v>803</v>
       </c>
       <c r="B656" t="s">
-        <v>806</v>
+        <v>804</v>
       </c>
     </row>
     <row r="657" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A657" t="s">
-        <v>807</v>
+        <v>805</v>
       </c>
       <c r="B657" t="s">
-        <v>808</v>
+        <v>806</v>
       </c>
     </row>
     <row r="658" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A658" t="s">
-        <v>809</v>
+        <v>807</v>
       </c>
       <c r="B658" t="s">
         <v>808</v>
@@ -8462,15 +8465,15 @@
     </row>
     <row r="659" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A659" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
       <c r="B659" t="s">
-        <v>811</v>
+        <v>808</v>
       </c>
     </row>
     <row r="660" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A660" t="s">
-        <v>812</v>
+        <v>810</v>
       </c>
       <c r="B660" t="s">
         <v>811</v>
@@ -8478,31 +8481,31 @@
     </row>
     <row r="661" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A661" t="s">
-        <v>813</v>
+        <v>812</v>
       </c>
       <c r="B661" t="s">
-        <v>814</v>
+        <v>811</v>
       </c>
     </row>
     <row r="662" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A662" t="s">
-        <v>815</v>
+        <v>813</v>
       </c>
       <c r="B662" t="s">
-        <v>816</v>
+        <v>814</v>
       </c>
     </row>
     <row r="663" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A663" t="s">
-        <v>817</v>
+        <v>815</v>
       </c>
       <c r="B663" t="s">
-        <v>818</v>
+        <v>816</v>
       </c>
     </row>
     <row r="664" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A664" t="s">
-        <v>819</v>
+        <v>817</v>
       </c>
       <c r="B664" t="s">
         <v>818</v>
@@ -8510,335 +8513,335 @@
     </row>
     <row r="665" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A665" t="s">
-        <v>820</v>
+        <v>819</v>
       </c>
       <c r="B665" t="s">
-        <v>519</v>
+        <v>818</v>
       </c>
     </row>
     <row r="666" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A666" t="s">
-        <v>821</v>
+        <v>820</v>
       </c>
       <c r="B666" t="s">
-        <v>822</v>
+        <v>519</v>
       </c>
     </row>
     <row r="667" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A667" t="s">
-        <v>823</v>
+        <v>821</v>
       </c>
       <c r="B667" t="s">
-        <v>35</v>
+        <v>822</v>
       </c>
     </row>
     <row r="668" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A668" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B668" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="669" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A669" t="s">
-        <v>825</v>
+        <v>824</v>
       </c>
       <c r="B669" t="s">
-        <v>3</v>
+        <v>37</v>
       </c>
     </row>
     <row r="670" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A670" t="s">
-        <v>826</v>
+        <v>825</v>
       </c>
       <c r="B670" t="s">
-        <v>81</v>
+        <v>3</v>
       </c>
     </row>
     <row r="671" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A671" t="s">
-        <v>827</v>
+        <v>826</v>
       </c>
       <c r="B671" t="s">
-        <v>708</v>
+        <v>81</v>
       </c>
     </row>
     <row r="672" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A672" t="s">
-        <v>828</v>
+        <v>827</v>
       </c>
       <c r="B672" t="s">
-        <v>523</v>
+        <v>708</v>
       </c>
     </row>
     <row r="673" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A673" t="s">
-        <v>829</v>
+        <v>828</v>
       </c>
       <c r="B673" t="s">
-        <v>44</v>
+        <v>523</v>
       </c>
     </row>
     <row r="674" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A674" t="s">
-        <v>830</v>
+        <v>829</v>
       </c>
       <c r="B674" t="s">
-        <v>5</v>
+        <v>44</v>
       </c>
     </row>
     <row r="675" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A675" t="s">
-        <v>831</v>
+        <v>830</v>
       </c>
       <c r="B675" t="s">
-        <v>72</v>
+        <v>5</v>
       </c>
     </row>
     <row r="676" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A676" t="s">
-        <v>832</v>
+        <v>831</v>
       </c>
       <c r="B676" t="s">
-        <v>140</v>
+        <v>72</v>
       </c>
     </row>
     <row r="677" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A677" t="s">
-        <v>833</v>
+        <v>832</v>
       </c>
       <c r="B677" t="s">
-        <v>179</v>
+        <v>140</v>
       </c>
     </row>
     <row r="678" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A678" t="s">
-        <v>834</v>
+        <v>833</v>
       </c>
       <c r="B678" t="s">
-        <v>698</v>
+        <v>179</v>
       </c>
     </row>
     <row r="679" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A679" t="s">
-        <v>835</v>
+        <v>834</v>
       </c>
       <c r="B679" t="s">
-        <v>374</v>
+        <v>698</v>
       </c>
     </row>
     <row r="680" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A680" t="s">
-        <v>836</v>
+        <v>835</v>
       </c>
       <c r="B680" t="s">
-        <v>190</v>
+        <v>374</v>
       </c>
     </row>
     <row r="681" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A681" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
       <c r="B681" t="s">
-        <v>575</v>
+        <v>190</v>
       </c>
     </row>
     <row r="682" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A682" t="s">
-        <v>838</v>
+        <v>837</v>
       </c>
       <c r="B682" t="s">
-        <v>543</v>
+        <v>575</v>
       </c>
     </row>
     <row r="683" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A683" t="s">
-        <v>839</v>
+        <v>838</v>
       </c>
       <c r="B683" t="s">
-        <v>452</v>
+        <v>543</v>
       </c>
     </row>
     <row r="684" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A684" t="s">
-        <v>840</v>
+        <v>839</v>
       </c>
       <c r="B684" t="s">
-        <v>509</v>
+        <v>452</v>
       </c>
     </row>
     <row r="685" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A685" t="s">
-        <v>841</v>
+        <v>840</v>
       </c>
       <c r="B685" t="s">
-        <v>599</v>
+        <v>509</v>
       </c>
     </row>
     <row r="686" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A686" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
       <c r="B686" t="s">
-        <v>49</v>
+        <v>599</v>
       </c>
     </row>
     <row r="687" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A687" t="s">
-        <v>843</v>
+        <v>842</v>
       </c>
       <c r="B687" t="s">
-        <v>844</v>
+        <v>49</v>
       </c>
     </row>
     <row r="688" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A688" t="s">
-        <v>845</v>
+        <v>843</v>
       </c>
       <c r="B688" t="s">
-        <v>846</v>
+        <v>844</v>
       </c>
     </row>
     <row r="689" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A689" t="s">
-        <v>847</v>
+        <v>845</v>
       </c>
       <c r="B689" t="s">
-        <v>844</v>
+        <v>846</v>
       </c>
     </row>
     <row r="690" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A690" t="s">
-        <v>848</v>
+        <v>847</v>
       </c>
       <c r="B690" t="s">
-        <v>13</v>
+        <v>844</v>
       </c>
     </row>
     <row r="691" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A691" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
       <c r="B691" t="s">
-        <v>844</v>
+        <v>13</v>
       </c>
     </row>
     <row r="692" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A692" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
       <c r="B692" t="s">
-        <v>846</v>
+        <v>844</v>
       </c>
     </row>
     <row r="693" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A693" t="s">
-        <v>851</v>
+        <v>850</v>
       </c>
       <c r="B693" t="s">
-        <v>844</v>
+        <v>846</v>
       </c>
     </row>
     <row r="694" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A694" t="s">
-        <v>852</v>
+        <v>851</v>
       </c>
       <c r="B694" t="s">
-        <v>728</v>
+        <v>844</v>
       </c>
     </row>
     <row r="695" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A695" t="s">
-        <v>853</v>
+        <v>852</v>
       </c>
       <c r="B695" t="s">
-        <v>691</v>
+        <v>728</v>
       </c>
     </row>
     <row r="696" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A696" t="s">
-        <v>854</v>
+        <v>853</v>
       </c>
       <c r="B696" t="s">
-        <v>209</v>
+        <v>691</v>
       </c>
     </row>
     <row r="697" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A697" t="s">
-        <v>855</v>
+        <v>854</v>
       </c>
       <c r="B697" t="s">
-        <v>856</v>
+        <v>209</v>
       </c>
     </row>
     <row r="698" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A698" t="s">
-        <v>857</v>
+        <v>855</v>
       </c>
       <c r="B698" t="s">
-        <v>858</v>
+        <v>856</v>
       </c>
     </row>
     <row r="699" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A699" t="s">
-        <v>859</v>
+        <v>857</v>
       </c>
       <c r="B699" t="s">
-        <v>860</v>
+        <v>858</v>
       </c>
     </row>
     <row r="700" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A700" t="s">
-        <v>861</v>
+        <v>859</v>
       </c>
       <c r="B700" t="s">
-        <v>69</v>
+        <v>860</v>
       </c>
     </row>
     <row r="701" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A701" t="s">
-        <v>755</v>
+        <v>861</v>
       </c>
       <c r="B701" t="s">
-        <v>754</v>
+        <v>69</v>
       </c>
     </row>
     <row r="702" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A702" t="s">
-        <v>862</v>
+        <v>755</v>
       </c>
       <c r="B702" t="s">
-        <v>45</v>
+        <v>754</v>
       </c>
     </row>
     <row r="703" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A703" t="s">
-        <v>863</v>
+        <v>862</v>
       </c>
       <c r="B703" t="s">
-        <v>864</v>
+        <v>45</v>
       </c>
     </row>
     <row r="704" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A704" t="s">
-        <v>865</v>
+        <v>863</v>
       </c>
       <c r="B704" t="s">
-        <v>617</v>
+        <v>864</v>
       </c>
     </row>
     <row r="705" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A705" t="s">
-        <v>866</v>
+        <v>865</v>
       </c>
       <c r="B705" t="s">
-        <v>51</v>
+        <v>617</v>
       </c>
     </row>
     <row r="706" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A706" t="s">
-        <v>867</v>
+        <v>866</v>
       </c>
       <c r="B706" t="s">
         <v>51</v>
@@ -8846,23 +8849,23 @@
     </row>
     <row r="707" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A707" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
       <c r="B707" t="s">
-        <v>869</v>
+        <v>51</v>
       </c>
     </row>
     <row r="708" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A708" t="s">
-        <v>870</v>
+        <v>868</v>
       </c>
       <c r="B708" t="s">
-        <v>864</v>
+        <v>869</v>
       </c>
     </row>
     <row r="709" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A709" t="s">
-        <v>871</v>
+        <v>870</v>
       </c>
       <c r="B709" t="s">
         <v>864</v>
@@ -8870,63 +8873,63 @@
     </row>
     <row r="710" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A710" t="s">
-        <v>872</v>
+        <v>871</v>
       </c>
       <c r="B710" t="s">
-        <v>732</v>
+        <v>864</v>
       </c>
     </row>
     <row r="711" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A711" t="s">
-        <v>873</v>
+        <v>872</v>
       </c>
       <c r="B711" t="s">
-        <v>69</v>
+        <v>732</v>
       </c>
     </row>
     <row r="712" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A712" t="s">
-        <v>874</v>
+        <v>873</v>
       </c>
       <c r="B712" t="s">
-        <v>3</v>
+        <v>69</v>
       </c>
     </row>
     <row r="713" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A713" t="s">
-        <v>875</v>
+        <v>874</v>
       </c>
       <c r="B713" t="s">
-        <v>876</v>
+        <v>3</v>
       </c>
     </row>
     <row r="714" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A714" t="s">
-        <v>877</v>
+        <v>875</v>
       </c>
       <c r="B714" t="s">
-        <v>878</v>
+        <v>876</v>
       </c>
     </row>
     <row r="715" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A715" t="s">
-        <v>879</v>
+        <v>877</v>
       </c>
       <c r="B715" t="s">
-        <v>818</v>
+        <v>878</v>
       </c>
     </row>
     <row r="716" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A716" t="s">
-        <v>880</v>
+        <v>879</v>
       </c>
       <c r="B716" t="s">
-        <v>881</v>
+        <v>818</v>
       </c>
     </row>
     <row r="717" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A717" t="s">
-        <v>882</v>
+        <v>880</v>
       </c>
       <c r="B717" t="s">
         <v>881</v>
@@ -8934,71 +8937,71 @@
     </row>
     <row r="718" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A718" t="s">
-        <v>883</v>
+        <v>882</v>
       </c>
       <c r="B718" t="s">
-        <v>749</v>
+        <v>881</v>
       </c>
     </row>
     <row r="719" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A719" t="s">
-        <v>884</v>
+        <v>883</v>
       </c>
       <c r="B719" t="s">
-        <v>856</v>
+        <v>749</v>
       </c>
     </row>
     <row r="720" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A720" t="s">
-        <v>885</v>
+        <v>884</v>
       </c>
       <c r="B720" t="s">
-        <v>844</v>
+        <v>856</v>
       </c>
     </row>
     <row r="721" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A721" t="s">
-        <v>886</v>
+        <v>885</v>
       </c>
       <c r="B721" t="s">
-        <v>76</v>
+        <v>844</v>
       </c>
     </row>
     <row r="722" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A722" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
       <c r="B722" t="s">
-        <v>888</v>
+        <v>76</v>
       </c>
     </row>
     <row r="723" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A723" t="s">
-        <v>889</v>
+        <v>887</v>
       </c>
       <c r="B723" t="s">
-        <v>869</v>
+        <v>888</v>
       </c>
     </row>
     <row r="724" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A724" t="s">
-        <v>890</v>
+        <v>889</v>
       </c>
       <c r="B724" t="s">
-        <v>51</v>
+        <v>869</v>
       </c>
     </row>
     <row r="725" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A725" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
       <c r="B725" t="s">
-        <v>881</v>
+        <v>51</v>
       </c>
     </row>
     <row r="726" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A726" t="s">
-        <v>892</v>
+        <v>891</v>
       </c>
       <c r="B726" t="s">
         <v>881</v>
@@ -9006,143 +9009,143 @@
     </row>
     <row r="727" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A727" t="s">
-        <v>893</v>
+        <v>892</v>
       </c>
       <c r="B727" t="s">
-        <v>844</v>
+        <v>881</v>
       </c>
     </row>
     <row r="728" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A728" t="s">
-        <v>894</v>
+        <v>893</v>
       </c>
       <c r="B728" t="s">
-        <v>69</v>
+        <v>844</v>
       </c>
     </row>
     <row r="729" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A729" t="s">
-        <v>895</v>
+        <v>894</v>
       </c>
       <c r="B729" t="s">
-        <v>881</v>
+        <v>69</v>
       </c>
     </row>
     <row r="730" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A730" t="s">
-        <v>896</v>
+        <v>895</v>
       </c>
       <c r="B730" t="s">
-        <v>57</v>
+        <v>881</v>
       </c>
     </row>
     <row r="731" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A731" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
       <c r="B731" t="s">
-        <v>7</v>
+        <v>57</v>
       </c>
     </row>
     <row r="732" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A732" t="s">
-        <v>898</v>
+        <v>897</v>
       </c>
       <c r="B732" t="s">
-        <v>51</v>
+        <v>7</v>
       </c>
     </row>
     <row r="733" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A733" t="s">
-        <v>899</v>
+        <v>898</v>
       </c>
       <c r="B733" t="s">
-        <v>864</v>
+        <v>51</v>
       </c>
     </row>
     <row r="734" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A734" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
       <c r="B734" t="s">
-        <v>69</v>
+        <v>864</v>
       </c>
     </row>
     <row r="735" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A735" t="s">
-        <v>901</v>
+        <v>900</v>
       </c>
       <c r="B735" t="s">
-        <v>479</v>
+        <v>69</v>
       </c>
     </row>
     <row r="736" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A736" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
       <c r="B736" t="s">
-        <v>864</v>
+        <v>479</v>
       </c>
     </row>
     <row r="737" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A737" t="s">
-        <v>903</v>
+        <v>902</v>
       </c>
       <c r="B737" t="s">
-        <v>881</v>
+        <v>864</v>
       </c>
     </row>
     <row r="738" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A738" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
       <c r="B738" t="s">
-        <v>115</v>
+        <v>881</v>
       </c>
     </row>
     <row r="739" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A739" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
       <c r="B739" t="s">
-        <v>728</v>
+        <v>115</v>
       </c>
     </row>
     <row r="740" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A740" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
       <c r="B740" t="s">
-        <v>190</v>
+        <v>728</v>
       </c>
     </row>
     <row r="741" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A741" t="s">
-        <v>907</v>
+        <v>906</v>
       </c>
       <c r="B741" t="s">
-        <v>51</v>
+        <v>190</v>
       </c>
     </row>
     <row r="742" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A742" t="s">
-        <v>908</v>
+        <v>907</v>
       </c>
       <c r="B742" t="s">
-        <v>7</v>
+        <v>51</v>
       </c>
     </row>
     <row r="743" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A743" t="s">
-        <v>909</v>
+        <v>908</v>
       </c>
       <c r="B743" t="s">
-        <v>57</v>
+        <v>7</v>
       </c>
     </row>
     <row r="744" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A744" t="s">
-        <v>910</v>
+        <v>909</v>
       </c>
       <c r="B744" t="s">
         <v>57</v>
@@ -9150,39 +9153,39 @@
     </row>
     <row r="745" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A745" t="s">
-        <v>911</v>
+        <v>910</v>
       </c>
       <c r="B745" t="s">
-        <v>844</v>
+        <v>57</v>
       </c>
     </row>
     <row r="746" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A746" t="s">
-        <v>912</v>
+        <v>911</v>
       </c>
       <c r="B746" t="s">
-        <v>153</v>
+        <v>844</v>
       </c>
     </row>
     <row r="747" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A747" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
       <c r="B747" t="s">
-        <v>914</v>
+        <v>153</v>
       </c>
     </row>
     <row r="748" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A748" t="s">
-        <v>915</v>
+        <v>913</v>
       </c>
       <c r="B748" t="s">
-        <v>881</v>
+        <v>914</v>
       </c>
     </row>
     <row r="749" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A749" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
       <c r="B749" t="s">
         <v>881</v>
@@ -9190,63 +9193,63 @@
     </row>
     <row r="750" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A750" t="s">
-        <v>917</v>
+        <v>916</v>
       </c>
       <c r="B750" t="s">
-        <v>811</v>
+        <v>881</v>
       </c>
     </row>
     <row r="751" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A751" t="s">
-        <v>918</v>
+        <v>917</v>
       </c>
       <c r="B751" t="s">
-        <v>846</v>
+        <v>811</v>
       </c>
     </row>
     <row r="752" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A752" t="s">
-        <v>919</v>
+        <v>918</v>
       </c>
       <c r="B752" t="s">
-        <v>64</v>
+        <v>846</v>
       </c>
     </row>
     <row r="753" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A753" t="s">
-        <v>920</v>
+        <v>919</v>
       </c>
       <c r="B753" t="s">
-        <v>728</v>
+        <v>64</v>
       </c>
     </row>
     <row r="754" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A754" t="s">
-        <v>921</v>
+        <v>920</v>
       </c>
       <c r="B754" t="s">
-        <v>34</v>
+        <v>728</v>
       </c>
     </row>
     <row r="755" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A755" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="B755" t="s">
-        <v>71</v>
+        <v>34</v>
       </c>
     </row>
     <row r="756" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A756" t="s">
-        <v>587</v>
+        <v>922</v>
       </c>
       <c r="B756" t="s">
-        <v>587</v>
+        <v>71</v>
       </c>
     </row>
     <row r="757" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A757" t="s">
-        <v>923</v>
+        <v>587</v>
       </c>
       <c r="B757" t="s">
         <v>587</v>
@@ -9254,33 +9257,41 @@
     </row>
     <row r="758" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A758" t="s">
-        <v>924</v>
+        <v>923</v>
       </c>
       <c r="B758" t="s">
-        <v>925</v>
+        <v>587</v>
       </c>
     </row>
     <row r="759" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A759" t="s">
-        <v>926</v>
+        <v>924</v>
       </c>
       <c r="B759" t="s">
-        <v>185</v>
+        <v>925</v>
       </c>
     </row>
     <row r="760" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A760" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="B760" t="s">
-        <v>54</v>
+        <v>185</v>
       </c>
     </row>
     <row r="761" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A761" t="s">
+        <v>927</v>
+      </c>
+      <c r="B761" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="762" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A762" t="s">
         <v>928</v>
       </c>
-      <c r="B761" t="s">
+      <c r="B762" t="s">
         <v>42</v>
       </c>
     </row>

</xml_diff>